<commit_message>
Demasiadas cosasa para hacer un buen commit
</commit_message>
<xml_diff>
--- a/public/archivos/tarifario.xlsx
+++ b/public/archivos/tarifario.xlsx
@@ -11,12 +11,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>tarifario</t>
-  </si>
-  <si>
-    <t>Este es un ejemplo de tarifario</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Cantidad en stock</t>
+  </si>
+  <si>
+    <t>Precio de venta</t>
+  </si>
+  <si>
+    <t>FIL001</t>
+  </si>
+  <si>
+    <t>Filtro de Aceite Premium</t>
+  </si>
+  <si>
+    <t>FP-1000</t>
+  </si>
+  <si>
+    <t>BAT002</t>
+  </si>
+  <si>
+    <t>Batería 12V 60Ah</t>
+  </si>
+  <si>
+    <t>BT-6000</t>
+  </si>
+  <si>
+    <t>DIS003</t>
+  </si>
+  <si>
+    <t>Juego de Discos de Freno</t>
+  </si>
+  <si>
+    <t>DF-2023</t>
+  </si>
+  <si>
+    <t>BUF004</t>
+  </si>
+  <si>
+    <t>Pastillas de Freno Delanteras</t>
+  </si>
+  <si>
+    <t>PF-D500</t>
+  </si>
+  <si>
+    <t>ACE005</t>
+  </si>
+  <si>
+    <t>Aceite Sintético 5W30</t>
+  </si>
+  <si>
+    <t>OIL-S5W30</t>
+  </si>
+  <si>
+    <t>FAR006</t>
+  </si>
+  <si>
+    <t>Faro Delantero Izquierdo</t>
+  </si>
+  <si>
+    <t>FD-450</t>
+  </si>
+  <si>
+    <t>COR007</t>
+  </si>
+  <si>
+    <t>Correa de Distribución</t>
+  </si>
+  <si>
+    <t>CD-789</t>
+  </si>
+  <si>
+    <t>AMO008</t>
+  </si>
+  <si>
+    <t>Amortiguador Trasero</t>
+  </si>
+  <si>
+    <t>AT-980</t>
+  </si>
+  <si>
+    <t>BOM009</t>
+  </si>
+  <si>
+    <t>Bomba de Agua</t>
+  </si>
+  <si>
+    <t>BA-350</t>
+  </si>
+  <si>
+    <t>BUJ010</t>
+  </si>
+  <si>
+    <t>Bujía de Encendido</t>
+  </si>
+  <si>
+    <t>BE-112</t>
   </si>
 </sst>
 </file>
@@ -31,9 +130,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,8 +143,22 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
@@ -54,8 +167,8 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -280,6 +393,185 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>55.99</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>199.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>320.75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>87.25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>210.9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>115.3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>275.6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>199.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>32.75</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>